<commit_message>
updated biofab container signatures
</commit_message>
<xml_diff>
--- a/scratch/biofab-sample-objects.xlsx
+++ b/scratch/biofab-sample-objects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danyfu/Documents/bio-circuit/aq-data-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danyfu/Documents/bio-circuit/crucible/scratch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2E2B94-E8C0-2A40-8B15-C581B78CFB2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793C813F-AF8E-174B-B5CA-ADC061018FB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36760" yWindow="560" windowWidth="36240" windowHeight="18600" xr2:uid="{2DE4FFE6-46AA-964F-BC5A-EB64A4A67A85}"/>
+    <workbookView xWindow="-38400" yWindow="580" windowWidth="36240" windowHeight="19300" xr2:uid="{2DE4FFE6-46AA-964F-BC5A-EB64A4A67A85}"/>
   </bookViews>
   <sheets>
     <sheet name="containers" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="750">
   <si>
     <t>500mL bottle</t>
   </si>
@@ -2156,9 +2156,6 @@
     <t>15mL</t>
   </si>
   <si>
-    <t>plant</t>
-  </si>
-  <si>
     <t>lentivirus container</t>
   </si>
   <si>
@@ -2168,9 +2165,6 @@
     <t>screw cap</t>
   </si>
   <si>
-    <t>container_type</t>
-  </si>
-  <si>
     <t>container</t>
   </si>
   <si>
@@ -2198,9 +2192,6 @@
     <t>tissue</t>
   </si>
   <si>
-    <t>leaf discs</t>
-  </si>
-  <si>
     <t>hydra dish</t>
   </si>
   <si>
@@ -2247,6 +2238,48 @@
   </si>
   <si>
     <t>1.8mL</t>
+  </si>
+  <si>
+    <t>container_attr</t>
+  </si>
+  <si>
+    <t>seeds</t>
+  </si>
+  <si>
+    <t>arabidopsis</t>
+  </si>
+  <si>
+    <t>arabidopsis-T1</t>
+  </si>
+  <si>
+    <t>plant-agrobacterium</t>
+  </si>
+  <si>
+    <t>n-benthamiana</t>
+  </si>
+  <si>
+    <t>arabidopsis-T2</t>
+  </si>
+  <si>
+    <t>arabidopsis-seedling</t>
+  </si>
+  <si>
+    <t>arabidopsis-T1-seedling</t>
+  </si>
+  <si>
+    <t>arabidopsis-T2-seedling</t>
+  </si>
+  <si>
+    <t>arabidopsis-T3-seedling</t>
+  </si>
+  <si>
+    <t>leaf disc</t>
+  </si>
+  <si>
+    <t>n-benthamiana-seedlings</t>
+  </si>
+  <si>
+    <t>slot</t>
   </si>
 </sst>
 </file>
@@ -2280,7 +2313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2302,6 +2335,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2333,7 +2372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2353,6 +2392,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2670,15 +2710,16 @@
   <dimension ref="A1:I199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D204" sqref="D204"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -2690,10 +2731,10 @@
         <v>597</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>712</v>
+        <v>736</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>628</v>
@@ -2705,10 +2746,10 @@
         <v>620</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>596</v>
@@ -2855,7 +2896,7 @@
       <c r="A10" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="15" t="s">
         <v>625</v>
       </c>
       <c r="C10" t="s">
@@ -2913,7 +2954,7 @@
         <v>623</v>
       </c>
       <c r="G13" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>244</v>
@@ -2941,7 +2982,7 @@
         <v>622</v>
       </c>
       <c r="C15" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E15" t="s">
         <v>626</v>
@@ -3022,6 +3063,9 @@
       <c r="B20" t="s">
         <v>600</v>
       </c>
+      <c r="C20" t="s">
+        <v>749</v>
+      </c>
       <c r="I20" s="2" t="s">
         <v>294</v>
       </c>
@@ -3498,6 +3542,9 @@
       <c r="B51" t="s">
         <v>622</v>
       </c>
+      <c r="C51" t="s">
+        <v>706</v>
+      </c>
       <c r="E51" t="s">
         <v>707</v>
       </c>
@@ -3509,9 +3556,17 @@
       <c r="A52" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="6" t="s">
         <v>598</v>
       </c>
+      <c r="C52" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
       <c r="I52" s="2" t="s">
         <v>430</v>
       </c>
@@ -3623,17 +3678,15 @@
       <c r="A59" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
       <c r="I59" s="2" t="s">
         <v>347</v>
       </c>
@@ -3643,10 +3696,10 @@
         <v>411</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
+      </c>
+      <c r="C60" t="s">
+        <v>743</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -3662,10 +3715,10 @@
         <v>402</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
+      </c>
+      <c r="C61" t="s">
+        <v>738</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -3681,10 +3734,10 @@
         <v>410</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
+      </c>
+      <c r="C62" t="s">
+        <v>744</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -3700,10 +3753,10 @@
         <v>390</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
+      </c>
+      <c r="C63" t="s">
+        <v>744</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -3719,10 +3772,10 @@
         <v>388</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
+      </c>
+      <c r="C64" t="s">
+        <v>745</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3738,10 +3791,10 @@
         <v>397</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
+      </c>
+      <c r="C65" t="s">
+        <v>746</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -3757,10 +3810,10 @@
         <v>400</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>719</v>
+        <v>717</v>
+      </c>
+      <c r="C66" t="s">
+        <v>746</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3776,10 +3829,10 @@
         <v>382</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C67" s="3" t="s">
         <v>625</v>
+      </c>
+      <c r="C67" t="s">
+        <v>746</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -3951,7 +4004,7 @@
         <v>465</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -3968,7 +4021,7 @@
         <v>457</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -4045,7 +4098,7 @@
         <v>625</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -4102,7 +4155,7 @@
         <v>622</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3" t="s">
@@ -4119,10 +4172,10 @@
       <c r="A86" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C86" s="3"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -4136,17 +4189,17 @@
       <c r="A87" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="6" t="s">
         <v>624</v>
       </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3" t="s">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
       <c r="I87" s="2" t="s">
         <v>278</v>
       </c>
@@ -4174,17 +4227,17 @@
       <c r="A89" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="6" t="s">
         <v>624</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3" t="s">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
       <c r="I89" s="2" t="s">
         <v>553</v>
       </c>
@@ -4216,7 +4269,7 @@
         <v>625</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D91" s="3">
         <v>96</v>
@@ -4234,10 +4287,10 @@
         <v>395</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>717</v>
+        <v>738</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -4253,10 +4306,10 @@
         <v>392</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>718</v>
+        <v>739</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -4272,10 +4325,10 @@
         <v>393</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>738</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -4381,7 +4434,7 @@
         <v>698</v>
       </c>
       <c r="C101" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>547</v>
@@ -4391,17 +4444,15 @@
       <c r="A102" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B102" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
+      <c r="B102" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
       <c r="I102" s="2" t="s">
         <v>363</v>
       </c>
@@ -4411,10 +4462,10 @@
         <v>372</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>708</v>
+        <v>719</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>721</v>
+        <v>738</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
@@ -4430,7 +4481,7 @@
         <v>516</v>
       </c>
       <c r="B104" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>515</v>
@@ -4441,7 +4492,7 @@
         <v>517</v>
       </c>
       <c r="B105" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>517</v>
@@ -4508,7 +4559,7 @@
         <v>622</v>
       </c>
       <c r="C110" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E110" t="s">
         <v>623</v>
@@ -4525,7 +4576,7 @@
         <v>622</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3" t="s">
@@ -4543,7 +4594,7 @@
         <v>467</v>
       </c>
       <c r="B112" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>466</v>
@@ -4554,7 +4605,7 @@
         <v>469</v>
       </c>
       <c r="B113" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>468</v>
@@ -4565,7 +4616,7 @@
         <v>461</v>
       </c>
       <c r="B114" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>460</v>
@@ -4576,7 +4627,7 @@
         <v>463</v>
       </c>
       <c r="B115" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>462</v>
@@ -4587,7 +4638,7 @@
         <v>471</v>
       </c>
       <c r="B116" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>470</v>
@@ -4649,7 +4700,7 @@
         <v>622</v>
       </c>
       <c r="C120" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E120" t="s">
         <v>626</v>
@@ -4929,7 +4980,7 @@
         <v>459</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -5085,10 +5136,10 @@
         <v>408</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>717</v>
+        <v>748</v>
       </c>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
@@ -5110,7 +5161,7 @@
         <v>623</v>
       </c>
       <c r="G148" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="I148" s="2" t="s">
         <v>582</v>
@@ -5141,13 +5192,13 @@
         <v>622</v>
       </c>
       <c r="C150" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E150" t="s">
         <v>623</v>
       </c>
       <c r="G150" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="I150" s="2" t="s">
         <v>574</v>
@@ -5249,10 +5300,10 @@
         <v>605</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>708</v>
+        <v>725</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>728</v>
+        <v>737</v>
       </c>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
@@ -5267,17 +5318,15 @@
       <c r="A157" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B157" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="3"/>
-      <c r="H157" s="3"/>
+      <c r="B157" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6"/>
+      <c r="H157" s="6"/>
       <c r="I157" s="2" t="s">
         <v>492</v>
       </c>
@@ -5312,7 +5361,7 @@
         <v>698</v>
       </c>
       <c r="C160" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>580</v>
@@ -5359,10 +5408,10 @@
         <v>485</v>
       </c>
       <c r="B164" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E164" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="I164" s="2" t="s">
         <v>484</v>
@@ -5373,10 +5422,10 @@
         <v>489</v>
       </c>
       <c r="B165" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E165" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="I165" s="2" t="s">
         <v>488</v>
@@ -5387,10 +5436,10 @@
         <v>487</v>
       </c>
       <c r="B166" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E166" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="I166" s="2" t="s">
         <v>486</v>
@@ -5477,10 +5526,10 @@
         <v>407</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
+      </c>
+      <c r="C172" t="s">
+        <v>738</v>
       </c>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
@@ -5496,10 +5545,10 @@
         <v>406</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
+      </c>
+      <c r="C173" t="s">
+        <v>739</v>
       </c>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
@@ -5515,9 +5564,11 @@
         <v>380</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C174" s="3"/>
+        <v>732</v>
+      </c>
+      <c r="C174" t="s">
+        <v>740</v>
+      </c>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
@@ -5532,10 +5583,10 @@
         <v>404</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
+      </c>
+      <c r="C175" t="s">
+        <v>741</v>
       </c>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
@@ -5551,10 +5602,10 @@
         <v>386</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
+      </c>
+      <c r="C176" t="s">
+        <v>739</v>
       </c>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
@@ -5570,10 +5621,10 @@
         <v>384</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>708</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
+      </c>
+      <c r="C177" t="s">
+        <v>742</v>
       </c>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
@@ -5603,7 +5654,7 @@
         <v>514</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
@@ -5647,9 +5698,15 @@
       <c r="A182" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B182" t="s">
-        <v>736</v>
-      </c>
+      <c r="B182" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="3"/>
       <c r="I182" s="2" t="s">
         <v>377</v>
       </c>
@@ -5658,9 +5715,15 @@
       <c r="A183" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B183" t="s">
-        <v>737</v>
-      </c>
+      <c r="B183" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
       <c r="I183" s="2" t="s">
         <v>490</v>
       </c>
@@ -5779,12 +5842,17 @@
       <c r="A191" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="B191" t="s">
-        <v>737</v>
-      </c>
-      <c r="F191" t="s">
-        <v>738</v>
-      </c>
+      <c r="B191" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="G191" s="6"/>
+      <c r="H191" s="6"/>
       <c r="I191" s="2" t="s">
         <v>543</v>
       </c>
@@ -5931,7 +5999,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>